<commit_message>
Add Wireframe for login page
</commit_message>
<xml_diff>
--- a/CLC_Milestone_1/CST-247-RS-SprintProductLogTemplate.xlsx
+++ b/CLC_Milestone_1/CST-247-RS-SprintProductLogTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Reps\GCU_CST247_CLC_Project\CLC_Milestone_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBEF51F-E351-4015-B946-38FEDAD84742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2412C04-7A13-4A4A-99C9-BD826448171C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26670" yWindow="1485" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Milestone Burndown" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
   <si>
     <t>User Stories</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Analyze Minesweeper code</t>
   </si>
   <si>
-    <t>As a dev group we would like a centeralized location for code and project files for collaboration and version control.</t>
-  </si>
-  <si>
     <t>Git server/ Create folder "Planning &amp; Design"</t>
   </si>
   <si>
@@ -220,6 +217,36 @@
   </si>
   <si>
     <t>LOW</t>
+  </si>
+  <si>
+    <t>Stephan</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>As a dev group we would like a centralized location for code and project files for collaboration and version control.</t>
+  </si>
+  <si>
+    <t>Tim/Stephan</t>
   </si>
 </sst>
 </file>
@@ -547,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -582,22 +609,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -609,21 +620,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -641,23 +637,11 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -683,11 +667,86 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -965,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F613DAAF-1369-4D8B-B35C-ADAF989D329E}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +1035,10 @@
     <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" customWidth="1"/>
+    <col min="6" max="8" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="13" width="9.28515625" customWidth="1"/>
     <col min="14" max="14" width="14.5703125" customWidth="1"/>
     <col min="15" max="15" width="10.28515625" customWidth="1"/>
     <col min="16" max="16" width="9.7109375" customWidth="1"/>
@@ -989,1262 +1051,1294 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="23"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="17"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="23"/>
-    </row>
-    <row r="3" spans="1:16" s="38" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" s="27" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="36" t="s">
+      <c r="L3" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="35" t="s">
+      <c r="N3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="37"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="26"/>
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="24">
+      <c r="A4" s="16"/>
+      <c r="B4" s="18">
         <v>1</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27">
+      <c r="E4" s="20"/>
+      <c r="F4" s="50">
+        <v>2</v>
+      </c>
+      <c r="G4" s="50">
+        <v>0</v>
+      </c>
+      <c r="H4" s="50">
+        <v>0</v>
+      </c>
+      <c r="I4" s="50">
+        <v>0</v>
+      </c>
+      <c r="J4" s="50">
+        <v>0</v>
+      </c>
+      <c r="K4" s="50">
+        <v>0</v>
+      </c>
+      <c r="L4" s="50">
+        <v>2</v>
+      </c>
+      <c r="M4" s="50">
+        <v>0</v>
+      </c>
+      <c r="N4" s="51">
+        <f>F4-(SUM(G4:M4))</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="16"/>
+      <c r="P4" s="17"/>
+    </row>
+    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="18">
+        <v>2</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="50">
         <v>1</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G5" s="50">
+        <v>1</v>
+      </c>
+      <c r="H5" s="50">
         <v>0</v>
       </c>
-      <c r="H4" s="27">
+      <c r="I5" s="50">
         <v>0</v>
       </c>
-      <c r="I4" s="27">
+      <c r="J5" s="50">
         <v>0</v>
       </c>
-      <c r="J4" s="27">
+      <c r="K5" s="50">
         <v>0</v>
       </c>
-      <c r="K4" s="27">
+      <c r="L5" s="50">
         <v>0</v>
       </c>
-      <c r="L4" s="27">
+      <c r="M5" s="50">
         <v>0</v>
       </c>
-      <c r="M4" s="27">
+      <c r="N5" s="51">
+        <f t="shared" ref="N5:N15" si="0">F5-(SUM(G5:M5))</f>
         <v>0</v>
       </c>
-      <c r="N4" s="28">
+      <c r="O5" s="16"/>
+      <c r="P5" s="17"/>
+    </row>
+    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="18">
+        <v>3</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="50">
         <v>1</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="23"/>
-    </row>
-    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="24">
+      <c r="G6" s="50">
+        <v>1</v>
+      </c>
+      <c r="H6" s="50">
+        <v>0</v>
+      </c>
+      <c r="I6" s="50">
+        <v>0</v>
+      </c>
+      <c r="J6" s="50">
+        <v>0</v>
+      </c>
+      <c r="K6" s="50">
+        <v>0</v>
+      </c>
+      <c r="L6" s="50">
+        <v>0</v>
+      </c>
+      <c r="M6" s="50">
+        <v>0</v>
+      </c>
+      <c r="N6" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="18">
+        <v>4</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="50">
+        <v>1</v>
+      </c>
+      <c r="G7" s="50">
+        <v>1</v>
+      </c>
+      <c r="H7" s="50">
+        <v>0</v>
+      </c>
+      <c r="I7" s="50">
+        <v>0</v>
+      </c>
+      <c r="J7" s="50">
+        <v>0</v>
+      </c>
+      <c r="K7" s="50">
+        <v>0</v>
+      </c>
+      <c r="L7" s="50">
+        <v>0</v>
+      </c>
+      <c r="M7" s="50">
+        <v>0</v>
+      </c>
+      <c r="N7" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16"/>
+      <c r="P7" s="17"/>
+    </row>
+    <row r="8" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="50">
+        <v>1</v>
+      </c>
+      <c r="G8" s="50">
+        <v>1</v>
+      </c>
+      <c r="H8" s="50">
+        <v>0</v>
+      </c>
+      <c r="I8" s="50">
+        <v>0</v>
+      </c>
+      <c r="J8" s="50">
+        <v>0</v>
+      </c>
+      <c r="K8" s="50">
+        <v>0</v>
+      </c>
+      <c r="L8" s="50">
+        <v>0</v>
+      </c>
+      <c r="M8" s="50">
+        <v>0</v>
+      </c>
+      <c r="N8" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16"/>
+      <c r="P8" s="17"/>
+    </row>
+    <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="18">
+        <v>5</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="50">
+        <v>1</v>
+      </c>
+      <c r="G9" s="50">
+        <v>1</v>
+      </c>
+      <c r="H9" s="50">
+        <v>0</v>
+      </c>
+      <c r="I9" s="50">
+        <v>0</v>
+      </c>
+      <c r="J9" s="50">
+        <v>0</v>
+      </c>
+      <c r="K9" s="50">
+        <v>0</v>
+      </c>
+      <c r="L9" s="50">
+        <v>0</v>
+      </c>
+      <c r="M9" s="50">
+        <v>0</v>
+      </c>
+      <c r="N9" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="16"/>
+      <c r="P9" s="17"/>
+    </row>
+    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="50">
         <v>2</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>25</v>
+      <c r="G10" s="50">
+        <v>0</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="27">
+      <c r="H10" s="50">
         <v>1</v>
       </c>
-      <c r="G5" s="27">
+      <c r="I10" s="50">
         <v>1</v>
       </c>
-      <c r="H5" s="27">
+      <c r="J10" s="50">
         <v>0</v>
       </c>
-      <c r="I5" s="27">
+      <c r="K10" s="50">
         <v>0</v>
       </c>
-      <c r="J5" s="27">
+      <c r="L10" s="50">
         <v>0</v>
       </c>
-      <c r="K5" s="27">
+      <c r="M10" s="50">
         <v>0</v>
       </c>
-      <c r="L5" s="27">
+      <c r="N10" s="51">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M5" s="27">
+      <c r="O10" s="16"/>
+      <c r="P10" s="17"/>
+    </row>
+    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="18">
+        <v>6</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="50">
+        <v>2</v>
+      </c>
+      <c r="G11" s="50">
+        <v>1</v>
+      </c>
+      <c r="H11" s="50">
         <v>0</v>
       </c>
-      <c r="N5" s="28">
+      <c r="I11" s="50">
         <v>0</v>
       </c>
-      <c r="O5" s="22"/>
-      <c r="P5" s="23"/>
-    </row>
-    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="24">
+      <c r="J11" s="50">
+        <v>1</v>
+      </c>
+      <c r="K11" s="50">
+        <v>0</v>
+      </c>
+      <c r="L11" s="50">
+        <v>0</v>
+      </c>
+      <c r="M11" s="50">
+        <v>0</v>
+      </c>
+      <c r="N11" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="16"/>
+      <c r="P11" s="17"/>
+    </row>
+    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="50">
+        <v>1</v>
+      </c>
+      <c r="G12" s="50">
+        <v>0</v>
+      </c>
+      <c r="H12" s="50">
+        <v>0</v>
+      </c>
+      <c r="I12" s="50">
+        <v>0</v>
+      </c>
+      <c r="J12" s="50">
+        <v>0</v>
+      </c>
+      <c r="K12" s="50">
+        <v>0</v>
+      </c>
+      <c r="L12" s="50">
+        <v>1</v>
+      </c>
+      <c r="M12" s="50">
+        <v>0</v>
+      </c>
+      <c r="N12" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="16"/>
+      <c r="P12" s="17"/>
+    </row>
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="50">
         <v>3</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>28</v>
+      <c r="G13" s="50">
+        <v>0</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>29</v>
+      <c r="H13" s="50">
+        <v>0</v>
       </c>
-      <c r="E6" s="26" t="s">
-        <v>27</v>
+      <c r="I13" s="50">
+        <v>0</v>
       </c>
-      <c r="F6" s="27">
+      <c r="J13" s="50">
+        <v>0</v>
+      </c>
+      <c r="K13" s="50">
+        <v>0</v>
+      </c>
+      <c r="L13" s="50">
+        <v>3</v>
+      </c>
+      <c r="M13" s="50">
+        <v>0</v>
+      </c>
+      <c r="N13" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="16"/>
+      <c r="P13" s="17"/>
+    </row>
+    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="50">
         <v>1</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G14" s="50">
         <v>1</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H14" s="50">
         <v>0</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I14" s="50">
         <v>0</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J14" s="50">
         <v>0</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K14" s="50">
         <v>0</v>
       </c>
-      <c r="L6" s="27">
+      <c r="L14" s="50">
         <v>0</v>
       </c>
-      <c r="M6" s="27">
+      <c r="M14" s="50">
         <v>0</v>
       </c>
-      <c r="N6" s="28">
+      <c r="N14" s="51">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O6" s="22"/>
-      <c r="P6" s="23"/>
-    </row>
-    <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="24">
-        <v>4</v>
+      <c r="O14" s="16"/>
+      <c r="P14" s="17"/>
+    </row>
+    <row r="15" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="18">
+        <v>7</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>30</v>
+      <c r="C15" s="19" t="s">
+        <v>46</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>31</v>
+      <c r="D15" s="19" t="s">
+        <v>47</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>27</v>
+      <c r="E15" s="20" t="s">
+        <v>59</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F15" s="50">
         <v>1</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G15" s="50">
+        <v>0</v>
+      </c>
+      <c r="H15" s="50">
+        <v>0</v>
+      </c>
+      <c r="I15" s="50">
+        <v>0</v>
+      </c>
+      <c r="J15" s="50">
+        <v>0</v>
+      </c>
+      <c r="K15" s="50">
+        <v>0</v>
+      </c>
+      <c r="L15" s="50">
+        <v>0</v>
+      </c>
+      <c r="M15" s="50">
         <v>1</v>
       </c>
-      <c r="H7" s="27">
+      <c r="N15" s="51">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="27">
+      <c r="O15" s="16"/>
+      <c r="P15" s="17"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="52">
+        <v>13</v>
+      </c>
+      <c r="G16" s="52">
+        <v>11.14</v>
+      </c>
+      <c r="H16" s="52">
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="I16" s="52">
+        <v>7.43</v>
+      </c>
+      <c r="J16" s="52">
+        <v>5.57</v>
+      </c>
+      <c r="K16" s="52">
+        <v>3.71</v>
+      </c>
+      <c r="L16" s="52">
+        <v>1.86</v>
+      </c>
+      <c r="M16" s="52">
         <v>0</v>
       </c>
-      <c r="J7" s="27">
-        <v>0</v>
+      <c r="N16" s="53"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="17"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="39" t="s">
+        <v>49</v>
       </c>
-      <c r="K7" s="27">
-        <v>0</v>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="52">
+        <v>13</v>
       </c>
-      <c r="L7" s="27">
-        <v>0</v>
-      </c>
-      <c r="M7" s="27">
-        <v>0</v>
-      </c>
-      <c r="N7" s="28">
-        <v>0</v>
-      </c>
-      <c r="O7" s="22"/>
-      <c r="P7" s="23"/>
-    </row>
-    <row r="8" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="27">
-        <v>1</v>
-      </c>
-      <c r="G8" s="27">
-        <v>1</v>
-      </c>
-      <c r="H8" s="27">
-        <v>0</v>
-      </c>
-      <c r="I8" s="27">
-        <v>0</v>
-      </c>
-      <c r="J8" s="27">
-        <v>0</v>
-      </c>
-      <c r="K8" s="27">
-        <v>0</v>
-      </c>
-      <c r="L8" s="27">
-        <v>0</v>
-      </c>
-      <c r="M8" s="27">
-        <v>0</v>
-      </c>
-      <c r="N8" s="28">
-        <v>0</v>
-      </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="23"/>
-    </row>
-    <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="24">
-        <v>5</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="27">
-        <v>1</v>
-      </c>
-      <c r="G9" s="27">
-        <v>1</v>
-      </c>
-      <c r="H9" s="27">
-        <v>0</v>
-      </c>
-      <c r="I9" s="27">
-        <v>0</v>
-      </c>
-      <c r="J9" s="27">
-        <v>0</v>
-      </c>
-      <c r="K9" s="27">
-        <v>0</v>
-      </c>
-      <c r="L9" s="27">
-        <v>0</v>
-      </c>
-      <c r="M9" s="27">
-        <v>0</v>
-      </c>
-      <c r="N9" s="28">
-        <v>0</v>
-      </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="23"/>
-    </row>
-    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="27">
-        <v>1</v>
-      </c>
-      <c r="G10" s="27">
-        <v>0</v>
-      </c>
-      <c r="H10" s="27">
-        <v>0</v>
-      </c>
-      <c r="I10" s="27">
-        <v>0</v>
-      </c>
-      <c r="J10" s="27">
-        <v>0</v>
-      </c>
-      <c r="K10" s="27">
-        <v>0</v>
-      </c>
-      <c r="L10" s="27">
-        <v>0</v>
-      </c>
-      <c r="M10" s="27">
-        <v>0</v>
-      </c>
-      <c r="N10" s="28">
-        <v>1</v>
-      </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="23"/>
-    </row>
-    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="24">
-        <v>6</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="27">
-        <v>2</v>
-      </c>
-      <c r="G11" s="27">
-        <v>1</v>
-      </c>
-      <c r="H11" s="27">
-        <v>0</v>
-      </c>
-      <c r="I11" s="27">
-        <v>0</v>
-      </c>
-      <c r="J11" s="27">
-        <v>0</v>
-      </c>
-      <c r="K11" s="27">
-        <v>0</v>
-      </c>
-      <c r="L11" s="27">
-        <v>0</v>
-      </c>
-      <c r="M11" s="27">
-        <v>0</v>
-      </c>
-      <c r="N11" s="28">
-        <v>1</v>
-      </c>
-      <c r="O11" s="22"/>
-      <c r="P11" s="23"/>
-    </row>
-    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="27">
-        <v>1</v>
-      </c>
-      <c r="G12" s="27">
-        <v>0</v>
-      </c>
-      <c r="H12" s="27">
-        <v>0</v>
-      </c>
-      <c r="I12" s="27">
-        <v>0</v>
-      </c>
-      <c r="J12" s="27">
-        <v>0</v>
-      </c>
-      <c r="K12" s="27">
-        <v>0</v>
-      </c>
-      <c r="L12" s="27">
-        <v>0</v>
-      </c>
-      <c r="M12" s="27">
-        <v>0</v>
-      </c>
-      <c r="N12" s="28">
-        <v>1</v>
-      </c>
-      <c r="O12" s="22"/>
-      <c r="P12" s="23"/>
-    </row>
-    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="27">
-        <v>1</v>
-      </c>
-      <c r="G13" s="27">
-        <v>0</v>
-      </c>
-      <c r="H13" s="27">
-        <v>0</v>
-      </c>
-      <c r="I13" s="27">
-        <v>0</v>
-      </c>
-      <c r="J13" s="27">
-        <v>0</v>
-      </c>
-      <c r="K13" s="27">
-        <v>0</v>
-      </c>
-      <c r="L13" s="27">
-        <v>0</v>
-      </c>
-      <c r="M13" s="27">
-        <v>0</v>
-      </c>
-      <c r="N13" s="28">
-        <v>1</v>
-      </c>
-      <c r="O13" s="22"/>
-      <c r="P13" s="23"/>
-    </row>
-    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="27">
-        <v>1</v>
-      </c>
-      <c r="G14" s="27">
-        <v>0</v>
-      </c>
-      <c r="H14" s="27">
-        <v>0</v>
-      </c>
-      <c r="I14" s="27">
-        <v>0</v>
-      </c>
-      <c r="J14" s="27">
-        <v>0</v>
-      </c>
-      <c r="K14" s="27">
-        <v>0</v>
-      </c>
-      <c r="L14" s="27">
-        <v>0</v>
-      </c>
-      <c r="M14" s="27">
-        <v>0</v>
-      </c>
-      <c r="N14" s="28">
-        <v>1</v>
-      </c>
-      <c r="O14" s="22"/>
-      <c r="P14" s="23"/>
-    </row>
-    <row r="15" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="24">
+      <c r="G17" s="52">
         <v>7</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27">
-        <v>1</v>
-      </c>
-      <c r="G15" s="27">
-        <v>0</v>
-      </c>
-      <c r="H15" s="27">
-        <v>0</v>
-      </c>
-      <c r="I15" s="27">
-        <v>0</v>
-      </c>
-      <c r="J15" s="27">
-        <v>0</v>
-      </c>
-      <c r="K15" s="27">
-        <v>0</v>
-      </c>
-      <c r="L15" s="27">
-        <v>0</v>
-      </c>
-      <c r="M15" s="27">
-        <v>0</v>
-      </c>
-      <c r="N15" s="28">
-        <v>1</v>
-      </c>
-      <c r="O15" s="22"/>
-      <c r="P15" s="23"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30">
-        <v>13</v>
-      </c>
-      <c r="G16" s="30">
-        <v>11.14</v>
-      </c>
-      <c r="H16" s="30">
-        <v>9.2899999999999991</v>
-      </c>
-      <c r="I16" s="30">
-        <v>7.43</v>
-      </c>
-      <c r="J16" s="30">
-        <v>5.57</v>
-      </c>
-      <c r="K16" s="30">
-        <v>3.71</v>
-      </c>
-      <c r="L16" s="30">
-        <v>1.86</v>
-      </c>
-      <c r="M16" s="30">
-        <v>0</v>
-      </c>
-      <c r="N16" s="31"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="23"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30">
-        <v>13</v>
-      </c>
-      <c r="G17" s="30">
+      <c r="H17" s="52">
         <v>7</v>
       </c>
-      <c r="H17" s="30">
+      <c r="I17" s="52">
         <v>7</v>
       </c>
-      <c r="I17" s="30">
+      <c r="J17" s="52">
         <v>7</v>
       </c>
-      <c r="J17" s="30">
+      <c r="K17" s="52">
         <v>7</v>
       </c>
-      <c r="K17" s="30">
+      <c r="L17" s="52">
         <v>7</v>
       </c>
-      <c r="L17" s="30">
+      <c r="M17" s="52">
         <v>7</v>
       </c>
-      <c r="M17" s="30">
-        <v>7</v>
-      </c>
-      <c r="N17" s="31"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="23"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="17"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="23"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="17"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="23"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="17"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="23"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="17"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="23"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="17"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="23"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="17"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="23"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="17"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="23"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="17"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="23"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="17"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="23"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="17"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="23"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="17"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="23"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="17"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="23"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="17"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="23"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="17"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="23"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="17"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="23"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="17"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="23"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="17"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="23"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="17"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="23"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="17"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="23"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="17"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="23"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="17"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="23"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="17"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="22"/>
-      <c r="P39" s="23"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="17"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="23"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="17"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="22"/>
-      <c r="P41" s="23"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="17"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="23"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="17"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="22"/>
-      <c r="P43" s="23"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="17"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="23"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="17"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="22"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="23"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="17"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="23"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="17"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="23"/>
-      <c r="L47" s="23"/>
-      <c r="M47" s="23"/>
-      <c r="N47" s="23"/>
-      <c r="O47" s="23"/>
-      <c r="P47" s="23"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="23"/>
-      <c r="L48" s="23"/>
-      <c r="M48" s="23"/>
-      <c r="N48" s="23"/>
-      <c r="O48" s="23"/>
-      <c r="P48" s="23"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="23"/>
-      <c r="M49" s="23"/>
-      <c r="N49" s="23"/>
-      <c r="O49" s="23"/>
-      <c r="P49" s="23"/>
+      <c r="A49" s="17"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="23"/>
-      <c r="L50" s="23"/>
-      <c r="M50" s="23"/>
-      <c r="N50" s="23"/>
-      <c r="O50" s="23"/>
-      <c r="P50" s="23"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2252,6 +2346,16 @@
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
   </mergeCells>
+  <conditionalFormatting sqref="N4:N15">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>1</formula>
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>-100</formula>
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2261,7 +2365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2060"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2279,14 +2383,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>51</v>
+      <c r="A1" s="43" t="s">
+        <v>50</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2295,11 +2399,11 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
       <c r="G2" s="5"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -25039,7 +25143,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="44" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
@@ -25050,382 +25154,382 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="1:9" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
+        <v>1</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44" t="s">
-        <v>0</v>
+      <c r="C4" s="32" t="s">
+        <v>53</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-    </row>
-    <row r="3" spans="1:9" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
-        <v>1</v>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33" t="s">
+        <v>54</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
         <v>2</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="B5" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
         <v>3</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
         <v>4</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
         <v>5</v>
       </c>
-      <c r="F3" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="52" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="46">
-        <v>1</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-    </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="46">
-        <v>2</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="46">
-        <v>3</v>
-      </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="46">
-        <v>4</v>
-      </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="46">
-        <v>5</v>
-      </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -25437,24 +25541,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9FDC2B66788A044965A7B8958E6244A" ma:contentTypeVersion="1251" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c2c36359d71eb747fbb188f75fc8d29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="d6188da8-f31e-469a-aed4-03a23c44e36a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="08acee74153637279a480e75df712a71" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25643,25 +25729,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A856C235-C1E3-486A-AF6F-91B1EB05F3BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5499EA-2107-4096-9690-EDC799091AC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347394F-0C4E-4E34-9270-1B2FF1850191}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25678,4 +25764,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5499EA-2107-4096-9690-EDC799091AC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A856C235-C1E3-486A-AF6F-91B1EB05F3BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>